<commit_message>
Update Matriz Vagas de emprego.xlsx
</commit_message>
<xml_diff>
--- a/Matriz Vagas de emprego.xlsx
+++ b/Matriz Vagas de emprego.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizh\OneDrive\Área de Trabalho\DEV\Projetos\Projetos Python\TRABALHO FINAL\CadastroDeVagasDeEmprego_TrabalhoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCE7D805-4687-44B4-BE42-B6F98D41428C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15269AA7-AB07-480F-AA85-CC34F1086443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{087893D2-8499-40DA-A095-52AE442563D6}"/>
+    <workbookView xWindow="1785" yWindow="1395" windowWidth="21600" windowHeight="11835" xr2:uid="{087893D2-8499-40DA-A095-52AE442563D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Titulo da Vaga</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Quantidade de vagas</t>
+  </si>
+  <si>
+    <t>Não utilizado</t>
   </si>
 </sst>
 </file>
@@ -357,71 +360,74 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -430,7 +436,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -485,19 +494,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{69B3DD28-A8F0-403F-9F28-FCC7879EEC18}" name="Tabela1" displayName="Tabela1" ref="D3:M13" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{69B3DD28-A8F0-403F-9F28-FCC7879EEC18}" name="Tabela1" displayName="Tabela1" ref="D3:M13" totalsRowShown="0" dataDxfId="10">
   <autoFilter ref="D3:M13" xr:uid="{69B3DD28-A8F0-403F-9F28-FCC7879EEC18}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{918D911D-66AA-41C6-814F-4BE4ABD2305F}" name="Java" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{52E1DD2C-D9B2-4F5F-A794-DD5779426D62}" name="Python" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{B2E623EB-6E88-4A7E-B1B6-BDEEE04BFF12}" name="SQL" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{91ED7361-80A0-4032-9E3C-3CCECA50AE36}" name="Git" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{BBF371DE-A3CB-45C2-9719-15EE102B3B61}" name="Spring" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{E7CE07C4-6D5E-4805-85D9-7DAA646E55F4}" name="Figma" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{3EB6498B-5B87-4514-8D0B-71E8B769690F}" name="Adobe XD" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{84045039-EAE9-4B6D-A51B-F03B8AF95424}" name="Comunicação" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{863AA3DB-ADF3-48C9-B76E-BFEB6A36E2CC}" name="Power BI" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{E8060E4F-F3EF-425A-B1C0-C4FF974210E3}" name="Linux" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{918D911D-66AA-41C6-814F-4BE4ABD2305F}" name="Java" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{52E1DD2C-D9B2-4F5F-A794-DD5779426D62}" name="Python" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{B2E623EB-6E88-4A7E-B1B6-BDEEE04BFF12}" name="SQL" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{91ED7361-80A0-4032-9E3C-3CCECA50AE36}" name="Git" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{BBF371DE-A3CB-45C2-9719-15EE102B3B61}" name="Spring" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{E7CE07C4-6D5E-4805-85D9-7DAA646E55F4}" name="Figma" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{3EB6498B-5B87-4514-8D0B-71E8B769690F}" name="Adobe XD" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{84045039-EAE9-4B6D-A51B-F03B8AF95424}" name="Comunicação" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{863AA3DB-ADF3-48C9-B76E-BFEB6A36E2CC}" name="Power BI" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{E8060E4F-F3EF-425A-B1C0-C4FF974210E3}" name="Linux" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -822,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ECCB2E9-D4AC-4D5E-B7BB-323464C7A434}">
   <dimension ref="B2:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,299 +845,311 @@
   <sheetData>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="15"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="4"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="4"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="15"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="4"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="4"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="15"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="4"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="4"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="15"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="4"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="4"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="15"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="4"/>
     </row>
     <row r="13" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="6"/>
     </row>
     <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="26" t="s">
+      <c r="C17" s="24"/>
+      <c r="D17" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="19"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
+      <c r="E17" s="20"/>
+      <c r="F17" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="27"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="20"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
+      <c r="C18" s="22"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="21"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="10" t="s">
+      <c r="C19" s="16"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="20"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="s">
+      <c r="C20" s="14"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="21"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
+      <c r="C21" s="16"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="20"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="9" t="s">
+      <c r="C22" s="14"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="21"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
+      <c r="C23" s="16"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="20"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="9" t="s">
+      <c r="C24" s="14"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="21"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="s">
+      <c r="C25" s="16"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="20"/>
-    </row>
-    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="11" t="s">
+      <c r="C26" s="14"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="23"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
+  <mergeCells count="34">
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
@@ -1145,18 +1166,11 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">

</xml_diff>